<commit_message>
Style - course front 완료
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munchanghyeon/PycharmProjects/2022-01-OSSP1-CodePirates-09/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimtaeuk/PycharmProjects/2022-01-OSSP1-CodePirates-09/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC71D0F5-39A2-8D4F-A384-6E59CFB1A70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B28A3ED-EF2A-954A-885E-47F796084A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16080" firstSheet="2" activeTab="8" xr2:uid="{6E62390C-CD6A-A842-95BF-41C492A543D2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" activeTab="11" xr2:uid="{6E62390C-CD6A-A842-95BF-41C492A543D2}"/>
   </bookViews>
   <sheets>
     <sheet name="충무로역.점심식사" sheetId="2" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="617">
   <si>
     <t>Column1</t>
   </si>
@@ -685,9 +685,6 @@
     <t xml:space="preserve"> 또보겠지떡볶이집 붕붕허니비점</t>
   </si>
   <si>
-    <t>동교동</t>
-  </si>
-  <si>
     <t>회전율이 엄청 빠릅니다..! 들어갔는데 5분도 안 되어서 나온 거 같아요! 그리고 5시에 갔을 땐 줄이 별로 없었는데 다먹고 나와서 보니까 줄이 길어지더라고요..? 갈거면 빨리 가</t>
   </si>
   <si>
@@ -1249,9 +1246,6 @@
     <t xml:space="preserve"> 멘야하나비 본점</t>
   </si>
   <si>
-    <t>송파동</t>
-  </si>
-  <si>
     <t>매장 방문 세 번, 배달 두 번. 코로나 창궐 이전엔 웨이팅 때문에 엄두도 못 내다가 한창 코로나로 난리일 때 첫 방문. 요즘은 주말엔 웨이팅이 말도 못하고, 평일 점심 때는</t>
   </si>
   <si>
@@ -1817,6 +1811,198 @@
   </si>
   <si>
     <t>https://d12zq4w4guyljn.cloudfront.net/pre_20220507071258_photo1_577e7ed4211d.jpg</t>
+  </si>
+  <si>
+    <t>서울 중구 수표로12길 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로12길 19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 수표로 42-9 2층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 마른내로 18 저동빌딩 지층 을지로술집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 수표로 48-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 충무로2길 28-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 충무로2길 32 제1호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 퇴계로 188</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 충무로7길 2 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 퇴계로27길 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 충무로2길 27-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 충무로5길 28 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 퇴계로 188 충무로역4번출구 바로앞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 퇴계로27길 39 2층 이층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 충무로7길 19 4층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 퇴계로32길 8 1,2층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 을지로12길 12 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 퇴계로 197 충무빌딩 지하 1012호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 수표로 26 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 수표로10길 19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 마른내로 62-1 2층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 필동로 32 낙원빌딩 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 수표로 42-21 3F~5F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 마포구 양화로19길 22-25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 와우산로29길 4-42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 와우산로29라길 26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 어울마당로 146</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 홍익로2길 23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 동교로34길 21 3, 4층 루나씨엘로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 동교로 225</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 어울마당로 136-13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 동교로25길 7 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 어울마당로 155-1 4층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 마포구 월드컵북로5가길 17 1층 슈아브</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 백제고분로45길 38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 올림픽로 269 잠실롯데캐슬 2층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 올림픽로 300 롯데월드몰 엔터테인먼트동 7층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 송파구 올림픽로 300 잠실 에비뉴엘 6층 롯데뮤지엄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 올림픽로 300 롯데월드몰 5층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 백제고분로45길 21-7 건물 전체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 오금로11길 14 별미곱창 본점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 송파구 올림픽로35가길 10 더샵스타파크상가 114호, 115호, 119호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 송파구 석촌호수로 284 지하104호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 종로구 자하문로24길 41-42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 을지로20길 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울특별시 중구 수표로 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울 중구 을지로12길 22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2217,10 +2403,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{0A94937D-02D8-E545-8CD5-AA90E2161C89}" name="data__13" displayName="data__13" ref="A1:D21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D21" xr:uid="{0A94937D-02D8-E545-8CD5-AA90E2161C89}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AB0FE93F-6345-5E46-BDBA-344AE3DDC6DC}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{40B82409-94AB-BC4C-B8F2-36CAD1DF502C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{17B4984C-3B1A-9D40-BF29-E12072ED1C18}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A96CA3FE-933E-9645-B480-35C036A2F5D7}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{AB0FE93F-6345-5E46-BDBA-344AE3DDC6DC}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{40B82409-94AB-BC4C-B8F2-36CAD1DF502C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{17B4984C-3B1A-9D40-BF29-E12072ED1C18}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A96CA3FE-933E-9645-B480-35C036A2F5D7}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2230,10 +2416,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C5D58EBA-A1C1-A342-A1DE-A00F63A3FD87}" name="data__12" displayName="data__12" ref="A1:D21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D21" xr:uid="{C5D58EBA-A1C1-A342-A1DE-A00F63A3FD87}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A29F1B51-6142-F747-9FDD-BACA17AA0190}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{56A173F1-65AC-6047-BCCA-7F1E623D1F31}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{5E9BC66A-6BD1-CE45-AF9E-ED722B761830}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2FCB482B-DA87-754D-BB1D-CD80AE0CD163}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A29F1B51-6142-F747-9FDD-BACA17AA0190}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{56A173F1-65AC-6047-BCCA-7F1E623D1F31}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5E9BC66A-6BD1-CE45-AF9E-ED722B761830}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{2FCB482B-DA87-754D-BB1D-CD80AE0CD163}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2295,10 +2481,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0528450B-4467-C348-88CC-A2CB81EBAF96}" name="data__8" displayName="data__8" ref="A1:D21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D21" xr:uid="{0528450B-4467-C348-88CC-A2CB81EBAF96}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ED65A24F-0E0A-144C-AD86-A6C4404E979F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{D50A99A6-9F65-FD4E-B807-293D62C7221C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{AACB222D-49EA-D741-85A2-5A51B0D42C78}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{4478EC71-20BA-594B-99E3-AC0298978812}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{ED65A24F-0E0A-144C-AD86-A6C4404E979F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{D50A99A6-9F65-FD4E-B807-293D62C7221C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{AACB222D-49EA-D741-85A2-5A51B0D42C78}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{4478EC71-20BA-594B-99E3-AC0298978812}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2308,10 +2494,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BA9D151C-B930-3B46-ACC3-84047337643C}" name="data__7" displayName="data__7" ref="A1:D21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D21" xr:uid="{BA9D151C-B930-3B46-ACC3-84047337643C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D4B31931-4650-3145-8232-C025A57332B4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C212D700-641E-694C-80EB-FB8B94A708ED}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{27812ECE-F1F4-FB42-A6FB-46C448B015D3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{E5B75172-2D90-3544-BF2A-A1EAACD4C9D4}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{D4B31931-4650-3145-8232-C025A57332B4}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{C212D700-641E-694C-80EB-FB8B94A708ED}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{27812ECE-F1F4-FB42-A6FB-46C448B015D3}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{E5B75172-2D90-3544-BF2A-A1EAACD4C9D4}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2643,7 +2829,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2673,7 +2859,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>613</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -2757,7 +2943,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>614</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -2869,7 +3055,7 @@
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>615</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>51</v>
@@ -2962,7 +3148,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2989,282 +3175,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3281,7 +3467,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3308,282 +3494,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>552</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -3599,8 +3785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CF64E6-646F-394D-B171-D0F49EE83EAE}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3627,282 +3813,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>476</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>497</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>503</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3919,7 +4105,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3949,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>613</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -4033,7 +4219,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>614</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>26</v>
@@ -4145,7 +4331,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>616</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>45</v>
@@ -4237,12 +4423,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81FEE48-A4B0-2A42-8E11-71F79612EA83}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.5703125" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4266,7 +4454,7 @@
         <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>569</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -4280,7 +4468,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>570</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>77</v>
@@ -4294,7 +4482,7 @@
         <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>571</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>80</v>
@@ -4308,7 +4496,7 @@
         <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>572</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -4322,7 +4510,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>573</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>86</v>
@@ -4336,7 +4524,7 @@
         <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>574</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>89</v>
@@ -4350,7 +4538,7 @@
         <v>91</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>575</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>92</v>
@@ -4364,7 +4552,7 @@
         <v>94</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>576</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>95</v>
@@ -4378,7 +4566,7 @@
         <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>577</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>98</v>
@@ -4392,7 +4580,7 @@
         <v>100</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>586</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>101</v>
@@ -4406,7 +4594,7 @@
         <v>103</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>584</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>104</v>
@@ -4420,7 +4608,7 @@
         <v>106</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>585</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>107</v>
@@ -4434,7 +4622,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>587</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>110</v>
@@ -4448,7 +4636,7 @@
         <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>588</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>113</v>
@@ -4462,7 +4650,7 @@
         <v>115</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>583</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>116</v>
@@ -4476,7 +4664,7 @@
         <v>118</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>582</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>119</v>
@@ -4490,7 +4678,7 @@
         <v>121</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>581</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>122</v>
@@ -4504,7 +4692,7 @@
         <v>124</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>580</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>125</v>
@@ -4518,7 +4706,7 @@
         <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>579</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>128</v>
@@ -4532,7 +4720,7 @@
         <v>130</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>578</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>131</v>
@@ -4554,7 +4742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33B6A2D-3065-CF49-8366-2355F2D25665}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -4583,7 +4773,7 @@
         <v>133</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>589</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>134</v>
@@ -4667,7 +4857,7 @@
         <v>148</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>590</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>149</v>
@@ -4779,7 +4969,7 @@
         <v>173</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>591</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>174</v>
@@ -4871,7 +5061,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14BC1AC0-8B8C-6A45-882A-DAAA51ECFE0F}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -4900,279 +5092,279 @@
         <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -5188,7 +5380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6363342-5EEC-DF4B-81FB-F21BEF5712F0}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -5217,279 +5411,279 @@
         <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -5506,7 +5700,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5533,282 +5727,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5825,7 +6019,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5852,282 +6046,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>363</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -6143,8 +6337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB84C680-377F-4749-990A-E890DDD2F76B}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -6171,282 +6365,282 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>416</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>419</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>423</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>446</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIN - Project done.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimtaeuk/PycharmProjects/2022-01-OSSP1-CodePirates-09/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B28A3ED-EF2A-954A-885E-47F796084A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C325AC-7D3D-F443-AF48-316B360C818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" activeTab="11" xr2:uid="{6E62390C-CD6A-A842-95BF-41C492A543D2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" activeTab="9" xr2:uid="{6E62390C-CD6A-A842-95BF-41C492A543D2}"/>
   </bookViews>
   <sheets>
     <sheet name="충무로역.점심식사" sheetId="2" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <sheet name="홍대입구역.술집" sheetId="8" r:id="rId7"/>
     <sheet name="홍대입구역.카페" sheetId="10" r:id="rId8"/>
     <sheet name="잠실역.점심식사" sheetId="11" r:id="rId9"/>
-    <sheet name="잠심역.저녁식사" sheetId="12" r:id="rId10"/>
+    <sheet name="잠실역.저녁식사" sheetId="12" r:id="rId10"/>
     <sheet name="잠실역.카페" sheetId="14" r:id="rId11"/>
     <sheet name="잠실역.술집" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="11" hidden="1">잠실역.술집!$A$1:$D$21</definedName>
+    <definedName name="ExternalData_1" localSheetId="9" hidden="1">잠실역.저녁식사!$A$1:$D$21</definedName>
     <definedName name="ExternalData_1" localSheetId="8" hidden="1">잠실역.점심식사!$A$1:$D$21</definedName>
-    <definedName name="ExternalData_1" localSheetId="9" hidden="1">잠심역.저녁식사!$A$1:$D$21</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">충무로역.저녁식사!$A$1:$D$21</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">충무로역.점심식사!$A$1:$D$21</definedName>
     <definedName name="ExternalData_1" localSheetId="3" hidden="1">충무로역.카페!$A$1:$D$21</definedName>
@@ -3147,8 +3147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA71021-D5F9-9945-B7AC-01D33B889E63}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3785,7 +3785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CF64E6-646F-394D-B171-D0F49EE83EAE}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>

</xml_diff>